<commit_message>
V1.5a production changes, change crystal to one with higher load abbilitys
</commit_message>
<xml_diff>
--- a/hardware/bill_of_materials/v1.5/MISRC V1.5.kicad_pcb_bom.xlsx
+++ b/hardware/bill_of_materials/v1.5/MISRC V1.5.kicad_pcb_bom.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\000 RF Decode Wiki GitHubs\0000 Github Atom Editing\MISRC\hardware\bill_of_materials\v1.5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F03B93-195E-496B-8835-15155158A9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4020" yWindow="4080" windowWidth="38700" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="BOM V1.5" sheetId="1" r:id="rId4"/>
+    <sheet name="BOM V1.5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="182">
   <si>
     <t>Designator</t>
   </si>
@@ -497,13 +506,14 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">-20 = 20msps / -40 = 40msps / -65 = 65msps </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF4D9EEF"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t>https://m.tb.cn/h.5tW5QqMkqOTZUye?tk=rmCIW9Fmz03</t>
     </r>
@@ -549,18 +559,6 @@
     <t>40Mhz</t>
   </si>
   <si>
-    <t>Oscillator_SMD_EuroQuartz_XO53-4Pin_5.0x3.2mm</t>
-  </si>
-  <si>
-    <t>XO32050UITA-40.000</t>
-  </si>
-  <si>
-    <t>Alternative: OT503240MJBA4SL</t>
-  </si>
-  <si>
-    <t>PCBWay Friendly Version v1.5</t>
-  </si>
-  <si>
     <t>Grand Total Parts: 192</t>
   </si>
   <si>
@@ -570,73 +568,106 @@
     <t>Allow Substitutes yes.</t>
   </si>
   <si>
-    <t>Date: 15.08.2024 (DD.MM.YYYY)</t>
-  </si>
-  <si>
     <t>Note: Mounting Holes 3.2mm M3</t>
+  </si>
+  <si>
+    <t>Oscillator XO91 4Pin 7.0x5.0mm</t>
+  </si>
+  <si>
+    <t>CB3LV-5I-40M0000</t>
+  </si>
+  <si>
+    <t>Date: 05.02.2025 (DD.MM.YYYY)</t>
+  </si>
+  <si>
+    <t>PCBWay Friendly Version v1.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0E9EFE"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF39AAF8"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF40B1FE"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF3DAFFD"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF4D9EEF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -644,7 +675,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -666,16 +697,26 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF343A3C"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF343A3C"/>
       </right>
@@ -685,86 +726,73 @@
       <bottom style="thin">
         <color rgb="FF343A3C"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -954,32 +982,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.38"/>
-    <col customWidth="1" min="2" max="2" width="14.0"/>
-    <col customWidth="1" min="3" max="3" width="30.5"/>
-    <col customWidth="1" min="4" max="4" width="41.63"/>
-    <col customWidth="1" min="5" max="5" width="11.25"/>
-    <col customWidth="1" min="6" max="6" width="27.0"/>
-    <col customWidth="1" min="7" max="7" width="23.13"/>
-    <col customWidth="1" min="8" max="8" width="39.25"/>
-    <col customWidth="1" min="9" max="9" width="48.13"/>
-    <col customWidth="1" min="12" max="12" width="34.0"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
+    <col min="9" max="9" width="48.140625" customWidth="1"/>
+    <col min="12" max="12" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,12 +1039,12 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="12.75">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
@@ -1030,12 +1063,12 @@
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="12.75">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
@@ -1057,12 +1090,12 @@
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="12.75">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>21</v>
@@ -1082,12 +1115,12 @@
       <c r="H4" s="6"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="12.75">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>25</v>
@@ -1107,12 +1140,12 @@
       <c r="H5" s="6"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
+    <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="7">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>28</v>
@@ -1131,12 +1164,12 @@
       </c>
       <c r="K6" s="13"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="12.75">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="7">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>31</v>
@@ -1155,12 +1188,12 @@
       </c>
       <c r="K7" s="13"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="12.75">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>34</v>
@@ -1179,12 +1212,12 @@
       </c>
       <c r="K8" s="11"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="12.75">
       <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>38</v>
@@ -1206,12 +1239,12 @@
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="12.75">
       <c r="A10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>42</v>
@@ -1230,12 +1263,12 @@
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="12.75">
       <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>45</v>
@@ -1254,12 +1287,12 @@
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="12.75">
       <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>25</v>
@@ -1278,12 +1311,12 @@
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="12.75">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>50</v>
@@ -1302,12 +1335,12 @@
       </c>
       <c r="K13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="12.75">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>54</v>
@@ -1329,12 +1362,12 @@
       </c>
       <c r="K14" s="9"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="12.75">
       <c r="A15" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>59</v>
@@ -1354,12 +1387,12 @@
       <c r="H15" s="6"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" ht="12.75">
       <c r="A16" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>63</v>
@@ -1371,19 +1404,19 @@
         <v>17</v>
       </c>
       <c r="F16" s="9">
-        <v>6.1300811121E10</v>
+        <v>61300811121</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" ht="12.75">
       <c r="A17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>66</v>
@@ -1395,7 +1428,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="9">
-        <v>6.1302021121E10</v>
+        <v>61302021121</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>13</v>
@@ -1405,12 +1438,12 @@
       </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" ht="12.75">
       <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>70</v>
@@ -1422,7 +1455,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="9">
-        <v>6.1302021121E10</v>
+        <v>61302021121</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>13</v>
@@ -1432,12 +1465,12 @@
       </c>
       <c r="K18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" ht="12.75">
       <c r="A19" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>72</v>
@@ -1456,12 +1489,12 @@
       </c>
       <c r="K19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" ht="12.75">
       <c r="A20" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>76</v>
@@ -1480,12 +1513,12 @@
       </c>
       <c r="K20" s="11"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" ht="12.75">
       <c r="A21" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B21" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>81</v>
@@ -1504,12 +1537,12 @@
       </c>
       <c r="K21" s="11"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" ht="12.75">
       <c r="A22" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B22" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>85</v>
@@ -1528,12 +1561,12 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" ht="12.75">
       <c r="A23" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>88</v>
@@ -1552,12 +1585,12 @@
       </c>
       <c r="K23" s="13"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" ht="12.75">
       <c r="A24" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>92</v>
@@ -1576,12 +1609,12 @@
       </c>
       <c r="K24" s="13"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" ht="12.75">
       <c r="A25" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>95</v>
@@ -1600,12 +1633,12 @@
       </c>
       <c r="K25" s="13"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" ht="12.75">
       <c r="A26" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B26" s="7">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>98</v>
@@ -1624,12 +1657,12 @@
       </c>
       <c r="K26" s="13"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" ht="12.75">
       <c r="A27" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B27" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>101</v>
@@ -1648,12 +1681,12 @@
       </c>
       <c r="K27" s="13"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" ht="12.75">
       <c r="A28" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B28" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>104</v>
@@ -1672,12 +1705,12 @@
       </c>
       <c r="K28" s="13"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" ht="12.75">
       <c r="A29" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B29" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>107</v>
@@ -1696,12 +1729,12 @@
       </c>
       <c r="K29" s="13"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" ht="12.75">
       <c r="A30" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>110</v>
@@ -1720,12 +1753,12 @@
       </c>
       <c r="K30" s="13"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" ht="12.75">
       <c r="A31" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B31" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>113</v>
@@ -1744,12 +1777,12 @@
       </c>
       <c r="K31" s="13"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" ht="12.75">
       <c r="A32" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B32" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>101</v>
@@ -1769,12 +1802,12 @@
       <c r="H32" s="6"/>
       <c r="K32" s="13"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" ht="12.75">
       <c r="A33" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B33" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>117</v>
@@ -1793,12 +1826,12 @@
       </c>
       <c r="K33" s="13"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" ht="12.75">
       <c r="A34" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B34" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>120</v>
@@ -1817,12 +1850,12 @@
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" ht="12.75">
       <c r="A35" s="6" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>123</v>
@@ -1841,12 +1874,12 @@
       </c>
       <c r="K35" s="13"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" ht="12.75">
       <c r="A36" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B36" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>88</v>
@@ -1865,12 +1898,12 @@
       </c>
       <c r="K36" s="11"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" ht="12.75">
       <c r="A37" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B37" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>130</v>
@@ -1889,12 +1922,12 @@
       </c>
       <c r="K37" s="11"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" ht="12.75">
       <c r="A38" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B38" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>134</v>
@@ -1913,12 +1946,12 @@
       </c>
       <c r="K38" s="9"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" ht="12.75">
       <c r="A39" s="6" t="s">
         <v>137</v>
       </c>
       <c r="B39" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>138</v>
@@ -1937,12 +1970,12 @@
       </c>
       <c r="K39" s="9"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" ht="12.75">
       <c r="A40" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B40" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>142</v>
@@ -1961,12 +1994,12 @@
       </c>
       <c r="K40" s="9"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" ht="12.75">
       <c r="A41" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B41" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>146</v>
@@ -1985,15 +2018,15 @@
       </c>
       <c r="K41" s="13"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:11" ht="12.75">
       <c r="A42" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B42" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="9">
-        <v>4043.0</v>
+        <v>4043</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>150</v>
@@ -2009,12 +2042,12 @@
       </c>
       <c r="K42" s="11"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" ht="12.75">
       <c r="A43" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B43" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>153</v>
@@ -2036,12 +2069,12 @@
       </c>
       <c r="K43" s="11"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:11" ht="12.75">
       <c r="A44" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B44" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>157</v>
@@ -2063,12 +2096,12 @@
       </c>
       <c r="K44" s="9"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:11" ht="12.75">
       <c r="A45" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B45" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>162</v>
@@ -2088,12 +2121,12 @@
       <c r="H45" s="6"/>
       <c r="K45" s="11"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:11" ht="12.75">
       <c r="A46" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B46" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>165</v>
@@ -2112,12 +2145,12 @@
       </c>
       <c r="K46" s="11"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:11" ht="12.75">
       <c r="A47" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B47" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>169</v>
@@ -2136,80 +2169,79 @@
       </c>
       <c r="K47" s="9"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:11" ht="12.75">
       <c r="A48" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B48" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>173</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>175</v>
+      <c r="F48" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H48" s="6"/>
+      <c r="K48" s="9"/>
+    </row>
+    <row r="49" spans="1:11" ht="12.75">
+      <c r="K49" s="11"/>
+    </row>
+    <row r="50" spans="1:11" ht="12.75">
+      <c r="A50" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="22.5" customHeight="1">
+      <c r="A51" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="14.25">
+      <c r="A52" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="14.25">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" ht="14.25">
+      <c r="A54" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="K48" s="9"/>
-    </row>
-    <row r="49">
-      <c r="K49" s="11"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="6" t="s">
+    </row>
+    <row r="55" spans="1:11" ht="14.25">
+      <c r="A55" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="12.75">
+      <c r="A56" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="51" ht="22.5" customHeight="1">
-      <c r="A51" s="19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="5"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" ht="178.5" customHeight="1"/>
+    <row r="57" spans="1:11" ht="178.5" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F4"/>
-    <hyperlink r:id="rId2" ref="F11"/>
-    <hyperlink r:id="rId3" ref="F12"/>
-    <hyperlink r:id="rId4" ref="H14"/>
-    <hyperlink r:id="rId5" ref="F26"/>
-    <hyperlink r:id="rId6" ref="H43"/>
-    <hyperlink r:id="rId7" ref="H44"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F26" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H43" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H44" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Amphenol SMA to generic SMA (901-144-8RFX is not in common cable use)
</commit_message>
<xml_diff>
--- a/hardware/bill_of_materials/v1.5/MISRC V1.5.kicad_pcb_bom.xlsx
+++ b/hardware/bill_of_materials/v1.5/MISRC V1.5.kicad_pcb_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\000 RF Decode Wiki GitHubs\0000 Github Atom Editing\MISRC\hardware\bill_of_materials\v1.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12186335-67A4-4510-979F-C312143BA1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D470EDFE-6B60-4303-87DC-32706A82A2FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="4080" windowWidth="38700" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,15 +185,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>Conn_01x01_Shielded</t>
-  </si>
-  <si>
-    <t>SMA_Amphenol_901-144_Vertical</t>
-  </si>
-  <si>
-    <t>901-144-8RFX</t>
-  </si>
-  <si>
     <t>https://m.tb.cn/h.5G8UUMPs4BD5jl0?tk=fbloW9FPomB</t>
   </si>
   <si>
@@ -581,6 +572,15 @@
   </si>
   <si>
     <t>Oscillator_XO91_4Pin_7.0x5.0mm</t>
+  </si>
+  <si>
+    <t>SMA_Vertical</t>
+  </si>
+  <si>
+    <t>SMA Vertical</t>
+  </si>
+  <si>
+    <t>BWSMA-KE-Z001</t>
   </si>
 </sst>
 </file>
@@ -994,8 +994,8 @@
   </sheetPr>
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1343,43 +1343,43 @@
         <v>1</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="12.75">
       <c r="A15" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="7">
         <v>2</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>13</v>
@@ -1389,16 +1389,16 @@
     </row>
     <row r="16" spans="1:11" ht="12.75">
       <c r="A16" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>17</v>
@@ -1413,16 +1413,16 @@
     </row>
     <row r="17" spans="1:11" ht="12.75">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" s="7">
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>17</v>
@@ -1434,22 +1434,22 @@
         <v>13</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="12.75">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" s="7">
         <v>1</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>17</v>
@@ -1461,28 +1461,28 @@
         <v>13</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="12.75">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="7">
         <v>2</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>13</v>
@@ -1491,94 +1491,94 @@
     </row>
     <row r="20" spans="1:11" ht="12.75">
       <c r="A20" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="12.75">
       <c r="A21" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B21" s="7">
         <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="12.75">
       <c r="A22" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B22" s="7">
         <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="12.75">
       <c r="A23" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" s="7">
         <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>13</v>
@@ -1587,22 +1587,22 @@
     </row>
     <row r="24" spans="1:11" ht="12.75">
       <c r="A24" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B24" s="7">
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>13</v>
@@ -1611,22 +1611,22 @@
     </row>
     <row r="25" spans="1:11" ht="12.75">
       <c r="A25" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25" s="7">
         <v>2</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>13</v>
@@ -1635,22 +1635,22 @@
     </row>
     <row r="26" spans="1:11" ht="12.75">
       <c r="A26" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B26" s="7">
         <v>10</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>13</v>
@@ -1659,22 +1659,22 @@
     </row>
     <row r="27" spans="1:11" ht="12.75">
       <c r="A27" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B27" s="7">
         <v>4</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>13</v>
@@ -1683,22 +1683,22 @@
     </row>
     <row r="28" spans="1:11" ht="12.75">
       <c r="A28" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B28" s="7">
         <v>4</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>13</v>
@@ -1707,22 +1707,22 @@
     </row>
     <row r="29" spans="1:11" ht="12.75">
       <c r="A29" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B29" s="7">
         <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>13</v>
@@ -1731,22 +1731,22 @@
     </row>
     <row r="30" spans="1:11" ht="12.75">
       <c r="A30" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B30" s="7">
         <v>6</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>13</v>
@@ -1755,22 +1755,22 @@
     </row>
     <row r="31" spans="1:11" ht="12.75">
       <c r="A31" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="7">
         <v>4</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>13</v>
@@ -1779,22 +1779,22 @@
     </row>
     <row r="32" spans="1:11" ht="12.75">
       <c r="A32" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B32" s="7">
         <v>4</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>13</v>
@@ -1804,22 +1804,22 @@
     </row>
     <row r="33" spans="1:11" ht="12.75">
       <c r="A33" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B33" s="7">
         <v>4</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>13</v>
@@ -1828,22 +1828,22 @@
     </row>
     <row r="34" spans="1:11" ht="12.75">
       <c r="A34" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B34" s="7">
         <v>4</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>13</v>
@@ -1852,22 +1852,22 @@
     </row>
     <row r="35" spans="1:11" ht="12.75">
       <c r="A35" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B35" s="7">
         <v>2</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>13</v>
@@ -1876,46 +1876,46 @@
     </row>
     <row r="36" spans="1:11" ht="12.75">
       <c r="A36" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36" s="7">
         <v>2</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="12.75">
       <c r="A37" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B37" s="7">
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>13</v>
@@ -1924,22 +1924,22 @@
     </row>
     <row r="38" spans="1:11" ht="12.75">
       <c r="A38" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B38" s="7">
         <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>13</v>
@@ -1948,22 +1948,22 @@
     </row>
     <row r="39" spans="1:11" ht="12.75">
       <c r="A39" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B39" s="7">
         <v>6</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>13</v>
@@ -1972,22 +1972,22 @@
     </row>
     <row r="40" spans="1:11" ht="12.75">
       <c r="A40" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B40" s="7">
         <v>2</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>13</v>
@@ -1996,22 +1996,22 @@
     </row>
     <row r="41" spans="1:11" ht="12.75">
       <c r="A41" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B41" s="7">
         <v>1</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>13</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="42" spans="1:11" ht="12.75">
       <c r="A42" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B42" s="7">
         <v>1</v>
@@ -2029,13 +2029,13 @@
         <v>4043</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>13</v>
@@ -2044,152 +2044,152 @@
     </row>
     <row r="43" spans="1:11" ht="12.75">
       <c r="A43" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B43" s="7">
         <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K43" s="11"/>
     </row>
     <row r="44" spans="1:11" ht="12.75">
       <c r="A44" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B44" s="7">
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" s="18" t="s">
         <v>157</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="12.75">
       <c r="A45" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B45" s="7">
         <v>4</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H45" s="6"/>
       <c r="K45" s="11"/>
     </row>
     <row r="46" spans="1:11" ht="12.75">
       <c r="A46" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B46" s="7">
         <v>1</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="1:11" ht="12.75">
       <c r="A47" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B47" s="7">
         <v>1</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="12.75">
       <c r="A48" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B48" s="7">
         <v>1</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H48" s="6"/>
       <c r="K48" s="9"/>
@@ -2199,17 +2199,17 @@
     </row>
     <row r="50" spans="1:11" ht="12.75">
       <c r="A50" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="22.5" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="14.25">
       <c r="A52" s="19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.25">
@@ -2217,17 +2217,17 @@
     </row>
     <row r="54" spans="1:11" ht="14.25">
       <c r="A54" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.25">
       <c r="A55" s="21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="12.75">
       <c r="A56" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="178.5" customHeight="1"/>

</xml_diff>